<commit_message>
update with new code
</commit_message>
<xml_diff>
--- a/Task_version_4/src/test/java/data/data.xlsx
+++ b/Task_version_4/src/test/java/data/data.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve"> Nacr city</t>
   </si>
   <si>
-    <t>zeinab21277@mailinator.com</t>
+    <t>zeinab2525@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding script for continue shopping
</commit_message>
<xml_diff>
--- a/Task_version_4/src/test/java/data/data.xlsx
+++ b/Task_version_4/src/test/java/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12816" windowHeight="5088"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t xml:space="preserve"> Nacr city</t>
   </si>
   <si>
-    <t>zeinab2525@mailinator.com</t>
+    <t>zeinabragab5new@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Make chromedriver path is dynamic
adding for class

	public static WebDriver driver;
	String driverPath=System.getProperty("user.dir")+"\\Drivers\\chromedriver.exe";
adding for function "SETUP"

		System.setProperty("webdriver.chrome.driver", driverPath);
</commit_message>
<xml_diff>
--- a/Task_version_4/src/test/java/data/data.xlsx
+++ b/Task_version_4/src/test/java/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="5088"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t xml:space="preserve"> Nacr city</t>
   </si>
   <si>
-    <t>zeinabragab5new@mailinator.com</t>
+    <t>zeinabtest77@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -375,14 +375,14 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>

</xml_diff>